<commit_message>
Formatação do Plano de Projeto
</commit_message>
<xml_diff>
--- a/docs/custo/estimativa-custo.xlsx
+++ b/docs/custo/estimativa-custo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desenvolvimento\FAI\rep-economundi\economundi\docs\custo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F606E1-E2AB-4343-A033-825682820A1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A70EFE0-0C1F-4045-88CD-DE622406CCA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCU-Fase x" sheetId="16" r:id="rId1"/>
@@ -19,12 +19,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PCU-Fase x'!$I$33:$I$35</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">'PCU-Fase x'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="146">
   <si>
     <t>Descrição</t>
   </si>
@@ -459,6 +467,9 @@
   </si>
   <si>
     <t>Gerenciar simulações</t>
+  </si>
+  <si>
+    <t>Portal EconoMundi</t>
   </si>
 </sst>
 </file>
@@ -1103,19 +1114,121 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1129,109 +1242,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1710,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U139"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A113" zoomScale="112" zoomScaleNormal="100" zoomScaleSheetLayoutView="112" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A118" zoomScale="112" zoomScaleNormal="100" zoomScaleSheetLayoutView="112" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1730,17 +1741,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="97"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="94"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="65"/>
@@ -1757,9 +1768,11 @@
       <c r="A3" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
+      <c r="B3" s="90" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="91"/>
+      <c r="D3" s="92"/>
       <c r="E3" s="58"/>
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
@@ -1781,7 +1794,9 @@
       <c r="A5" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="59"/>
+      <c r="B5" s="59">
+        <v>43598</v>
+      </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
@@ -1906,31 +1921,31 @@
       <c r="I14" s="39"/>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="116"/>
       <c r="I16" s="40" t="s">
         <v>2</v>
       </c>
@@ -1939,15 +1954,15 @@
       <c r="A17" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="117" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="104"/>
       <c r="I17" s="42">
         <v>1</v>
       </c>
@@ -1956,15 +1971,15 @@
       <c r="A18" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="79" t="s">
+      <c r="B18" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="104"/>
       <c r="I18" s="42">
         <v>2</v>
       </c>
@@ -1976,15 +1991,15 @@
       <c r="A19" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
       <c r="I19" s="42">
         <v>3</v>
       </c>
@@ -2012,10 +2027,10 @@
       <c r="A21" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="89" t="s">
+      <c r="B21" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="90"/>
+      <c r="C21" s="102"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="56" t="s">
@@ -2085,42 +2100,42 @@
       <c r="A29" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="75">
+      <c r="B29" s="113">
         <f>SUM(B22:C28)</f>
         <v>12</v>
       </c>
-      <c r="C29" s="76"/>
+      <c r="C29" s="114"/>
     </row>
     <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="95"/>
+      <c r="F31" s="95"/>
+      <c r="G31" s="95"/>
+      <c r="H31" s="95"/>
+      <c r="I31" s="95"/>
     </row>
     <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="118"/>
       <c r="I32" s="40" t="s">
         <v>2</v>
       </c>
@@ -2129,15 +2144,15 @@
       <c r="A33" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="70"/>
+      <c r="C33" s="104"/>
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="104"/>
       <c r="I33" s="42">
         <v>5</v>
       </c>
@@ -2146,15 +2161,15 @@
       <c r="A34" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
+      <c r="C34" s="104"/>
+      <c r="D34" s="104"/>
+      <c r="E34" s="104"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="104"/>
+      <c r="H34" s="104"/>
       <c r="I34" s="42">
         <v>10</v>
       </c>
@@ -2166,15 +2181,15 @@
       <c r="A35" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="104"/>
       <c r="I35" s="42">
         <v>15</v>
       </c>
@@ -2191,10 +2206,10 @@
       <c r="A37" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="89" t="s">
+      <c r="B37" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="90"/>
+      <c r="C37" s="102"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="H37" s="3"/>
@@ -2204,13 +2219,13 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="118" t="s">
+      <c r="A38" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="80">
+      <c r="B38" s="73">
         <v>5</v>
       </c>
-      <c r="C38" s="81"/>
+      <c r="C38" s="74"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -2220,7 +2235,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="118" t="s">
+      <c r="A39" s="70" t="s">
         <v>124</v>
       </c>
       <c r="B39" s="68">
@@ -2233,7 +2248,7 @@
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="118" t="s">
+      <c r="A40" s="70" t="s">
         <v>125</v>
       </c>
       <c r="B40" s="68">
@@ -2246,20 +2261,20 @@
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="118" t="s">
+      <c r="A41" s="70" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="80">
+      <c r="B41" s="73">
         <v>5</v>
       </c>
-      <c r="C41" s="81"/>
+      <c r="C41" s="74"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="118" t="s">
+      <c r="A42" s="70" t="s">
         <v>127</v>
       </c>
       <c r="B42" s="68">
@@ -2272,7 +2287,7 @@
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="118" t="s">
+      <c r="A43" s="70" t="s">
         <v>128</v>
       </c>
       <c r="B43" s="68">
@@ -2285,20 +2300,20 @@
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="118" t="s">
+      <c r="A44" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="B44" s="80">
+      <c r="B44" s="73">
         <v>5</v>
       </c>
-      <c r="C44" s="81"/>
+      <c r="C44" s="74"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="118" t="s">
+      <c r="A45" s="70" t="s">
         <v>130</v>
       </c>
       <c r="B45" s="68">
@@ -2311,7 +2326,7 @@
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="118" t="s">
+      <c r="A46" s="70" t="s">
         <v>131</v>
       </c>
       <c r="B46" s="68">
@@ -2324,20 +2339,20 @@
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="118" t="s">
+      <c r="A47" s="70" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="80">
+      <c r="B47" s="73">
         <v>5</v>
       </c>
-      <c r="C47" s="81"/>
+      <c r="C47" s="74"/>
       <c r="D47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="118" t="s">
+      <c r="A48" s="70" t="s">
         <v>133</v>
       </c>
       <c r="B48" s="68">
@@ -2350,7 +2365,7 @@
       <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A49" s="118" t="s">
+      <c r="A49" s="70" t="s">
         <v>134</v>
       </c>
       <c r="B49" s="68">
@@ -2363,20 +2378,20 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A50" s="118" t="s">
+      <c r="A50" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="80">
+      <c r="B50" s="73">
         <v>5</v>
       </c>
-      <c r="C50" s="81"/>
+      <c r="C50" s="74"/>
       <c r="D50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A51" s="118" t="s">
+      <c r="A51" s="70" t="s">
         <v>136</v>
       </c>
       <c r="B51" s="68">
@@ -2389,7 +2404,7 @@
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A52" s="118" t="s">
+      <c r="A52" s="70" t="s">
         <v>137</v>
       </c>
       <c r="B52" s="68">
@@ -2402,20 +2417,20 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A53" s="118" t="s">
+      <c r="A53" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="80">
+      <c r="B53" s="73">
         <v>5</v>
       </c>
-      <c r="C53" s="81"/>
+      <c r="C53" s="74"/>
       <c r="D53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A54" s="118" t="s">
+      <c r="A54" s="70" t="s">
         <v>139</v>
       </c>
       <c r="B54" s="68">
@@ -2428,7 +2443,7 @@
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A55" s="118" t="s">
+      <c r="A55" s="70" t="s">
         <v>140</v>
       </c>
       <c r="B55" s="68">
@@ -2441,20 +2456,20 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A56" s="118" t="s">
+      <c r="A56" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="B56" s="80">
+      <c r="B56" s="73">
         <v>5</v>
       </c>
-      <c r="C56" s="81"/>
+      <c r="C56" s="74"/>
       <c r="D56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A57" s="118" t="s">
+      <c r="A57" s="70" t="s">
         <v>142</v>
       </c>
       <c r="B57" s="68">
@@ -2467,7 +2482,7 @@
       <c r="H57" s="3"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A58" s="118" t="s">
+      <c r="A58" s="70" t="s">
         <v>143</v>
       </c>
       <c r="B58" s="68">
@@ -2480,7 +2495,7 @@
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A59" s="118" t="s">
+      <c r="A59" s="70" t="s">
         <v>144</v>
       </c>
       <c r="B59" s="68">
@@ -2496,11 +2511,11 @@
       <c r="A60" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="98">
+      <c r="B60" s="96">
         <f>SUM(B38:B59)</f>
         <v>110</v>
       </c>
-      <c r="C60" s="99"/>
+      <c r="C60" s="97"/>
       <c r="D60" s="3" t="s">
         <v>14</v>
       </c>
@@ -2525,11 +2540,11 @@
       <c r="A62" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="75">
+      <c r="B62" s="113">
         <f>B29+B60</f>
         <v>122</v>
       </c>
-      <c r="C62" s="76"/>
+      <c r="C62" s="114"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="9"/>
@@ -2554,17 +2569,17 @@
       <c r="U63" s="9"/>
     </row>
     <row r="64" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="73" t="s">
+      <c r="A64" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="B64" s="83"/>
-      <c r="C64" s="83"/>
-      <c r="D64" s="83"/>
-      <c r="E64" s="83"/>
-      <c r="F64" s="83"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="84"/>
-      <c r="I64" s="84"/>
+      <c r="B64" s="78"/>
+      <c r="C64" s="78"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="78"/>
+      <c r="F64" s="78"/>
+      <c r="G64" s="99"/>
+      <c r="H64" s="99"/>
+      <c r="I64" s="99"/>
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
@@ -2578,17 +2593,17 @@
       <c r="U64" s="9"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A65" s="70" t="s">
+      <c r="A65" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="70"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="70"/>
-      <c r="E65" s="70"/>
-      <c r="F65" s="70"/>
-      <c r="G65" s="70"/>
-      <c r="H65" s="70"/>
-      <c r="I65" s="70"/>
+      <c r="B65" s="104"/>
+      <c r="C65" s="104"/>
+      <c r="D65" s="104"/>
+      <c r="E65" s="104"/>
+      <c r="F65" s="104"/>
+      <c r="G65" s="104"/>
+      <c r="H65" s="104"/>
+      <c r="I65" s="104"/>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
@@ -2602,17 +2617,17 @@
       <c r="U65" s="9"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A66" s="70" t="s">
+      <c r="A66" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="70"/>
-      <c r="C66" s="70"/>
-      <c r="D66" s="70"/>
-      <c r="E66" s="70"/>
-      <c r="F66" s="70"/>
-      <c r="G66" s="70"/>
-      <c r="H66" s="70"/>
-      <c r="I66" s="70"/>
+      <c r="B66" s="104"/>
+      <c r="C66" s="104"/>
+      <c r="D66" s="104"/>
+      <c r="E66" s="104"/>
+      <c r="F66" s="104"/>
+      <c r="G66" s="104"/>
+      <c r="H66" s="104"/>
+      <c r="I66" s="104"/>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
@@ -2626,17 +2641,17 @@
       <c r="U66" s="9"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A67" s="70" t="s">
+      <c r="A67" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="B67" s="70"/>
-      <c r="C67" s="70"/>
-      <c r="D67" s="70"/>
-      <c r="E67" s="70"/>
-      <c r="F67" s="70"/>
-      <c r="G67" s="70"/>
-      <c r="H67" s="70"/>
-      <c r="I67" s="70"/>
+      <c r="B67" s="104"/>
+      <c r="C67" s="104"/>
+      <c r="D67" s="104"/>
+      <c r="E67" s="104"/>
+      <c r="F67" s="104"/>
+      <c r="G67" s="104"/>
+      <c r="H67" s="104"/>
+      <c r="I67" s="104"/>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
@@ -2650,17 +2665,17 @@
       <c r="U67" s="9"/>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A68" s="70" t="s">
+      <c r="A68" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="84"/>
-      <c r="C68" s="84"/>
-      <c r="D68" s="84"/>
-      <c r="E68" s="84"/>
-      <c r="F68" s="84"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="84"/>
-      <c r="I68" s="84"/>
+      <c r="B68" s="99"/>
+      <c r="C68" s="99"/>
+      <c r="D68" s="99"/>
+      <c r="E68" s="99"/>
+      <c r="F68" s="99"/>
+      <c r="G68" s="99"/>
+      <c r="H68" s="99"/>
+      <c r="I68" s="99"/>
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
@@ -2677,22 +2692,22 @@
       <c r="A69" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B69" s="82" t="s">
+      <c r="B69" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="82"/>
-      <c r="D69" s="82"/>
-      <c r="E69" s="82"/>
+      <c r="C69" s="109"/>
+      <c r="D69" s="109"/>
+      <c r="E69" s="109"/>
       <c r="F69" s="46" t="s">
         <v>2</v>
       </c>
       <c r="G69" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H69" s="73" t="s">
+      <c r="H69" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="I69" s="73"/>
+      <c r="I69" s="95"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
@@ -2709,23 +2724,23 @@
       <c r="A70" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="B70" s="70" t="s">
+      <c r="B70" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="70"/>
-      <c r="D70" s="70"/>
-      <c r="E70" s="70"/>
+      <c r="C70" s="104"/>
+      <c r="D70" s="104"/>
+      <c r="E70" s="104"/>
       <c r="F70" s="42">
         <v>2</v>
       </c>
       <c r="G70" s="55">
         <v>5</v>
       </c>
-      <c r="H70" s="85">
+      <c r="H70" s="110">
         <f>F70*G70</f>
         <v>10</v>
       </c>
-      <c r="I70" s="85"/>
+      <c r="I70" s="110"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
@@ -2742,23 +2757,23 @@
       <c r="A71" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B71" s="70" t="s">
+      <c r="B71" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="70"/>
-      <c r="D71" s="70"/>
-      <c r="E71" s="70"/>
+      <c r="C71" s="104"/>
+      <c r="D71" s="104"/>
+      <c r="E71" s="104"/>
       <c r="F71" s="42">
         <v>1</v>
       </c>
       <c r="G71" s="55">
         <v>5</v>
       </c>
-      <c r="H71" s="85">
+      <c r="H71" s="110">
         <f t="shared" ref="H71:H82" si="0">F71*G71</f>
         <v>5</v>
       </c>
-      <c r="I71" s="85"/>
+      <c r="I71" s="110"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
@@ -2775,23 +2790,23 @@
       <c r="A72" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B72" s="70" t="s">
+      <c r="B72" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="70"/>
-      <c r="D72" s="70"/>
-      <c r="E72" s="70"/>
+      <c r="C72" s="104"/>
+      <c r="D72" s="104"/>
+      <c r="E72" s="104"/>
       <c r="F72" s="42">
         <v>1</v>
       </c>
       <c r="G72" s="55">
         <v>4</v>
       </c>
-      <c r="H72" s="85">
+      <c r="H72" s="110">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I72" s="85"/>
+      <c r="I72" s="110"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
@@ -2808,23 +2823,23 @@
       <c r="A73" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B73" s="70" t="s">
+      <c r="B73" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="C73" s="70"/>
-      <c r="D73" s="70"/>
-      <c r="E73" s="70"/>
+      <c r="C73" s="104"/>
+      <c r="D73" s="104"/>
+      <c r="E73" s="104"/>
       <c r="F73" s="42">
         <v>1</v>
       </c>
       <c r="G73" s="55">
         <v>5</v>
       </c>
-      <c r="H73" s="85">
+      <c r="H73" s="110">
         <f>F73*G73</f>
         <v>5</v>
       </c>
-      <c r="I73" s="85"/>
+      <c r="I73" s="110"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -2841,23 +2856,23 @@
       <c r="A74" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B74" s="70" t="s">
+      <c r="B74" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="70"/>
-      <c r="D74" s="70"/>
-      <c r="E74" s="70"/>
+      <c r="C74" s="104"/>
+      <c r="D74" s="104"/>
+      <c r="E74" s="104"/>
       <c r="F74" s="42">
         <v>1</v>
       </c>
       <c r="G74" s="55">
         <v>3</v>
       </c>
-      <c r="H74" s="85">
+      <c r="H74" s="110">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I74" s="85"/>
+      <c r="I74" s="110"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="11"/>
@@ -2874,23 +2889,23 @@
       <c r="A75" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B75" s="70" t="s">
+      <c r="B75" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C75" s="70"/>
-      <c r="D75" s="70"/>
-      <c r="E75" s="70"/>
+      <c r="C75" s="104"/>
+      <c r="D75" s="104"/>
+      <c r="E75" s="104"/>
       <c r="F75" s="42">
         <v>0.5</v>
       </c>
       <c r="G75" s="55">
         <v>0</v>
       </c>
-      <c r="H75" s="85">
+      <c r="H75" s="110">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I75" s="85"/>
+      <c r="I75" s="110"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -2907,23 +2922,23 @@
       <c r="A76" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="70" t="s">
+      <c r="B76" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="C76" s="70"/>
-      <c r="D76" s="70"/>
-      <c r="E76" s="70"/>
+      <c r="C76" s="104"/>
+      <c r="D76" s="104"/>
+      <c r="E76" s="104"/>
       <c r="F76" s="42">
         <v>0.5</v>
       </c>
       <c r="G76" s="55">
         <v>5</v>
       </c>
-      <c r="H76" s="85">
+      <c r="H76" s="110">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="I76" s="85"/>
+      <c r="I76" s="110"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
@@ -2940,23 +2955,23 @@
       <c r="A77" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B77" s="70" t="s">
+      <c r="B77" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="C77" s="70"/>
-      <c r="D77" s="70"/>
-      <c r="E77" s="70"/>
+      <c r="C77" s="104"/>
+      <c r="D77" s="104"/>
+      <c r="E77" s="104"/>
       <c r="F77" s="42">
         <v>2</v>
       </c>
       <c r="G77" s="55">
         <v>4</v>
       </c>
-      <c r="H77" s="85">
+      <c r="H77" s="110">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I77" s="85"/>
+      <c r="I77" s="110"/>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
@@ -2973,23 +2988,23 @@
       <c r="A78" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B78" s="70" t="s">
+      <c r="B78" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="C78" s="70"/>
-      <c r="D78" s="70"/>
-      <c r="E78" s="70"/>
+      <c r="C78" s="104"/>
+      <c r="D78" s="104"/>
+      <c r="E78" s="104"/>
       <c r="F78" s="42">
         <v>1</v>
       </c>
       <c r="G78" s="55">
         <v>5</v>
       </c>
-      <c r="H78" s="85">
+      <c r="H78" s="110">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I78" s="85"/>
+      <c r="I78" s="110"/>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
@@ -3006,23 +3021,23 @@
       <c r="A79" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="70" t="s">
+      <c r="B79" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="C79" s="70"/>
-      <c r="D79" s="70"/>
-      <c r="E79" s="70"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="104"/>
+      <c r="E79" s="104"/>
       <c r="F79" s="42">
         <v>1</v>
       </c>
       <c r="G79" s="55">
         <v>1</v>
       </c>
-      <c r="H79" s="85">
+      <c r="H79" s="110">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I79" s="85"/>
+      <c r="I79" s="110"/>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
@@ -3039,23 +3054,23 @@
       <c r="A80" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B80" s="70" t="s">
+      <c r="B80" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="70"/>
-      <c r="D80" s="70"/>
-      <c r="E80" s="70"/>
+      <c r="C80" s="104"/>
+      <c r="D80" s="104"/>
+      <c r="E80" s="104"/>
       <c r="F80" s="42">
         <v>1</v>
       </c>
       <c r="G80" s="55">
         <v>2</v>
       </c>
-      <c r="H80" s="85">
+      <c r="H80" s="110">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I80" s="85"/>
+      <c r="I80" s="110"/>
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
       <c r="M80" s="9"/>
@@ -3072,23 +3087,23 @@
       <c r="A81" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B81" s="70" t="s">
+      <c r="B81" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="C81" s="70"/>
-      <c r="D81" s="70"/>
-      <c r="E81" s="70"/>
+      <c r="C81" s="104"/>
+      <c r="D81" s="104"/>
+      <c r="E81" s="104"/>
       <c r="F81" s="42">
         <v>1</v>
       </c>
       <c r="G81" s="55">
         <v>5</v>
       </c>
-      <c r="H81" s="85">
+      <c r="H81" s="110">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I81" s="85"/>
+      <c r="I81" s="110"/>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
@@ -3105,23 +3120,23 @@
       <c r="A82" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B82" s="70" t="s">
+      <c r="B82" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="70"/>
-      <c r="D82" s="70"/>
-      <c r="E82" s="70"/>
+      <c r="C82" s="104"/>
+      <c r="D82" s="104"/>
+      <c r="E82" s="104"/>
       <c r="F82" s="42">
         <v>1</v>
       </c>
       <c r="G82" s="55">
         <v>1</v>
       </c>
-      <c r="H82" s="85">
+      <c r="H82" s="110">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I82" s="85"/>
+      <c r="I82" s="110"/>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -3135,20 +3150,20 @@
       <c r="U82" s="9"/>
     </row>
     <row r="83" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="83" t="s">
+      <c r="A83" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="84"/>
-      <c r="C83" s="84"/>
-      <c r="D83" s="84"/>
-      <c r="E83" s="84"/>
-      <c r="F83" s="84"/>
-      <c r="G83" s="84"/>
-      <c r="H83" s="92">
+      <c r="B83" s="99"/>
+      <c r="C83" s="99"/>
+      <c r="D83" s="99"/>
+      <c r="E83" s="99"/>
+      <c r="F83" s="99"/>
+      <c r="G83" s="99"/>
+      <c r="H83" s="111">
         <f>0.6+(0.01*(SUM(H70:I82)))</f>
         <v>1.115</v>
       </c>
-      <c r="I83" s="92"/>
+      <c r="I83" s="111"/>
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
@@ -3183,17 +3198,17 @@
       <c r="U84" s="9"/>
     </row>
     <row r="85" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="73" t="s">
+      <c r="A85" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="83"/>
-      <c r="C85" s="83"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="84"/>
-      <c r="F85" s="84"/>
-      <c r="G85" s="84"/>
-      <c r="H85" s="84"/>
-      <c r="I85" s="84"/>
+      <c r="B85" s="78"/>
+      <c r="C85" s="78"/>
+      <c r="D85" s="78"/>
+      <c r="E85" s="99"/>
+      <c r="F85" s="99"/>
+      <c r="G85" s="99"/>
+      <c r="H85" s="99"/>
+      <c r="I85" s="99"/>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
@@ -3207,17 +3222,17 @@
       <c r="U85" s="9"/>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A86" s="70" t="s">
+      <c r="A86" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="70"/>
-      <c r="C86" s="70"/>
-      <c r="D86" s="70"/>
-      <c r="E86" s="70"/>
-      <c r="F86" s="70"/>
-      <c r="G86" s="70"/>
-      <c r="H86" s="84"/>
-      <c r="I86" s="84"/>
+      <c r="B86" s="104"/>
+      <c r="C86" s="104"/>
+      <c r="D86" s="104"/>
+      <c r="E86" s="104"/>
+      <c r="F86" s="104"/>
+      <c r="G86" s="104"/>
+      <c r="H86" s="99"/>
+      <c r="I86" s="99"/>
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
@@ -3231,17 +3246,17 @@
       <c r="U86" s="9"/>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A87" s="70" t="s">
+      <c r="A87" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="70"/>
-      <c r="C87" s="70"/>
-      <c r="D87" s="70"/>
-      <c r="E87" s="70"/>
-      <c r="F87" s="70"/>
-      <c r="G87" s="70"/>
-      <c r="H87" s="84"/>
-      <c r="I87" s="84"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="104"/>
+      <c r="D87" s="104"/>
+      <c r="E87" s="104"/>
+      <c r="F87" s="104"/>
+      <c r="G87" s="104"/>
+      <c r="H87" s="99"/>
+      <c r="I87" s="99"/>
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
@@ -3255,17 +3270,17 @@
       <c r="U87" s="9"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A88" s="70" t="s">
+      <c r="A88" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="B88" s="70"/>
-      <c r="C88" s="70"/>
-      <c r="D88" s="70"/>
-      <c r="E88" s="70"/>
-      <c r="F88" s="70"/>
-      <c r="G88" s="70"/>
-      <c r="H88" s="84"/>
-      <c r="I88" s="84"/>
+      <c r="B88" s="104"/>
+      <c r="C88" s="104"/>
+      <c r="D88" s="104"/>
+      <c r="E88" s="104"/>
+      <c r="F88" s="104"/>
+      <c r="G88" s="104"/>
+      <c r="H88" s="99"/>
+      <c r="I88" s="99"/>
       <c r="K88" s="9"/>
       <c r="L88" s="9"/>
       <c r="M88" s="9"/>
@@ -3279,17 +3294,17 @@
       <c r="U88" s="9"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A89" s="70" t="s">
+      <c r="A89" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
-      <c r="D89" s="70"/>
-      <c r="E89" s="70"/>
-      <c r="F89" s="70"/>
-      <c r="G89" s="70"/>
-      <c r="H89" s="84"/>
-      <c r="I89" s="84"/>
+      <c r="B89" s="104"/>
+      <c r="C89" s="104"/>
+      <c r="D89" s="104"/>
+      <c r="E89" s="104"/>
+      <c r="F89" s="104"/>
+      <c r="G89" s="104"/>
+      <c r="H89" s="99"/>
+      <c r="I89" s="99"/>
       <c r="K89" s="9"/>
       <c r="L89" s="9"/>
       <c r="M89" s="9"/>
@@ -3303,17 +3318,17 @@
       <c r="U89" s="9"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A90" s="70" t="s">
+      <c r="A90" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="B90" s="84"/>
-      <c r="C90" s="84"/>
-      <c r="D90" s="84"/>
-      <c r="E90" s="84"/>
-      <c r="F90" s="84"/>
-      <c r="G90" s="84"/>
-      <c r="H90" s="84"/>
-      <c r="I90" s="84"/>
+      <c r="B90" s="99"/>
+      <c r="C90" s="99"/>
+      <c r="D90" s="99"/>
+      <c r="E90" s="99"/>
+      <c r="F90" s="99"/>
+      <c r="G90" s="99"/>
+      <c r="H90" s="99"/>
+      <c r="I90" s="99"/>
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
@@ -3330,13 +3345,13 @@
       <c r="A91" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B91" s="82" t="s">
+      <c r="B91" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="C91" s="70"/>
-      <c r="D91" s="70"/>
-      <c r="E91" s="70"/>
-      <c r="F91" s="70"/>
+      <c r="C91" s="104"/>
+      <c r="D91" s="104"/>
+      <c r="E91" s="104"/>
+      <c r="F91" s="104"/>
       <c r="G91" s="46" t="s">
         <v>2</v>
       </c>
@@ -3362,13 +3377,13 @@
       <c r="A92" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B92" s="70" t="s">
+      <c r="B92" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="C92" s="70"/>
-      <c r="D92" s="70"/>
-      <c r="E92" s="70"/>
-      <c r="F92" s="70"/>
+      <c r="C92" s="104"/>
+      <c r="D92" s="104"/>
+      <c r="E92" s="104"/>
+      <c r="F92" s="104"/>
       <c r="G92" s="42">
         <v>1.5</v>
       </c>
@@ -3399,13 +3414,13 @@
       <c r="A93" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B93" s="70" t="s">
+      <c r="B93" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="C93" s="70"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="70"/>
-      <c r="F93" s="70"/>
+      <c r="C93" s="104"/>
+      <c r="D93" s="104"/>
+      <c r="E93" s="104"/>
+      <c r="F93" s="104"/>
       <c r="G93" s="42">
         <v>0.5</v>
       </c>
@@ -3425,13 +3440,13 @@
       <c r="A94" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B94" s="70" t="s">
+      <c r="B94" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C94" s="70"/>
-      <c r="D94" s="70"/>
-      <c r="E94" s="70"/>
-      <c r="F94" s="70"/>
+      <c r="C94" s="104"/>
+      <c r="D94" s="104"/>
+      <c r="E94" s="104"/>
+      <c r="F94" s="104"/>
       <c r="G94" s="42">
         <v>1</v>
       </c>
@@ -3451,13 +3466,13 @@
       <c r="A95" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B95" s="70" t="s">
+      <c r="B95" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="C95" s="70"/>
-      <c r="D95" s="70"/>
-      <c r="E95" s="70"/>
-      <c r="F95" s="70"/>
+      <c r="C95" s="104"/>
+      <c r="D95" s="104"/>
+      <c r="E95" s="104"/>
+      <c r="F95" s="104"/>
       <c r="G95" s="42">
         <v>0.5</v>
       </c>
@@ -3477,13 +3492,13 @@
       <c r="A96" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B96" s="70" t="s">
+      <c r="B96" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C96" s="70"/>
-      <c r="D96" s="70"/>
-      <c r="E96" s="70"/>
-      <c r="F96" s="70"/>
+      <c r="C96" s="104"/>
+      <c r="D96" s="104"/>
+      <c r="E96" s="104"/>
+      <c r="F96" s="104"/>
       <c r="G96" s="42">
         <v>1</v>
       </c>
@@ -3503,13 +3518,13 @@
       <c r="A97" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B97" s="91" t="s">
+      <c r="B97" s="112" t="s">
         <v>100</v>
       </c>
-      <c r="C97" s="70"/>
-      <c r="D97" s="70"/>
-      <c r="E97" s="70"/>
-      <c r="F97" s="70"/>
+      <c r="C97" s="104"/>
+      <c r="D97" s="104"/>
+      <c r="E97" s="104"/>
+      <c r="F97" s="104"/>
       <c r="G97" s="42">
         <v>2</v>
       </c>
@@ -3529,13 +3544,13 @@
       <c r="A98" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B98" s="70" t="s">
+      <c r="B98" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="70"/>
-      <c r="D98" s="70"/>
-      <c r="E98" s="70"/>
-      <c r="F98" s="70"/>
+      <c r="C98" s="104"/>
+      <c r="D98" s="104"/>
+      <c r="E98" s="104"/>
+      <c r="F98" s="104"/>
       <c r="G98" s="42">
         <v>-1</v>
       </c>
@@ -3555,13 +3570,13 @@
       <c r="A99" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="B99" s="70" t="s">
+      <c r="B99" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C99" s="70"/>
-      <c r="D99" s="70"/>
-      <c r="E99" s="70"/>
-      <c r="F99" s="70"/>
+      <c r="C99" s="104"/>
+      <c r="D99" s="104"/>
+      <c r="E99" s="104"/>
+      <c r="F99" s="104"/>
       <c r="G99" s="42">
         <v>-1</v>
       </c>
@@ -3578,16 +3593,16 @@
       </c>
     </row>
     <row r="100" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="83" t="s">
+      <c r="A100" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="B100" s="83"/>
-      <c r="C100" s="83"/>
-      <c r="D100" s="83"/>
-      <c r="E100" s="83"/>
-      <c r="F100" s="83"/>
-      <c r="G100" s="83"/>
-      <c r="H100" s="83"/>
+      <c r="B100" s="78"/>
+      <c r="C100" s="78"/>
+      <c r="D100" s="78"/>
+      <c r="E100" s="78"/>
+      <c r="F100" s="78"/>
+      <c r="G100" s="78"/>
+      <c r="H100" s="78"/>
       <c r="I100" s="18">
         <f>1.4+(-0.03*(SUM(I92:I99)))</f>
         <v>1.325</v>
@@ -3607,172 +3622,172 @@
       <c r="B103" s="13"/>
     </row>
     <row r="104" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="113" t="s">
+      <c r="A104" s="82" t="s">
         <v>108</v>
       </c>
-      <c r="B104" s="114"/>
-      <c r="C104" s="114"/>
-      <c r="D104" s="114"/>
-      <c r="E104" s="114"/>
-      <c r="F104" s="114"/>
-      <c r="G104" s="114"/>
-      <c r="H104" s="114"/>
-      <c r="I104" s="114"/>
+      <c r="B104" s="83"/>
+      <c r="C104" s="83"/>
+      <c r="D104" s="83"/>
+      <c r="E104" s="83"/>
+      <c r="F104" s="83"/>
+      <c r="G104" s="83"/>
+      <c r="H104" s="83"/>
+      <c r="I104" s="83"/>
     </row>
     <row r="105" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="115" t="s">
+      <c r="A105" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="B105" s="116"/>
-      <c r="C105" s="116"/>
-      <c r="D105" s="116"/>
-      <c r="E105" s="116"/>
-      <c r="F105" s="116"/>
-      <c r="G105" s="116"/>
-      <c r="H105" s="116"/>
-      <c r="I105" s="117"/>
+      <c r="B105" s="85"/>
+      <c r="C105" s="85"/>
+      <c r="D105" s="85"/>
+      <c r="E105" s="85"/>
+      <c r="F105" s="85"/>
+      <c r="G105" s="85"/>
+      <c r="H105" s="85"/>
+      <c r="I105" s="86"/>
     </row>
     <row r="106" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="109" t="s">
+      <c r="A106" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="B106" s="83"/>
-      <c r="C106" s="83"/>
-      <c r="D106" s="83"/>
-      <c r="E106" s="83"/>
-      <c r="F106" s="83"/>
-      <c r="G106" s="83"/>
-      <c r="H106" s="83"/>
-      <c r="I106" s="110"/>
+      <c r="B106" s="78"/>
+      <c r="C106" s="78"/>
+      <c r="D106" s="78"/>
+      <c r="E106" s="78"/>
+      <c r="F106" s="78"/>
+      <c r="G106" s="78"/>
+      <c r="H106" s="78"/>
+      <c r="I106" s="79"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A107" s="102" t="s">
+      <c r="A107" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="B107" s="70"/>
-      <c r="C107" s="70"/>
-      <c r="D107" s="70"/>
-      <c r="E107" s="70"/>
-      <c r="F107" s="70"/>
-      <c r="G107" s="70"/>
-      <c r="H107" s="70"/>
-      <c r="I107" s="103"/>
+      <c r="B107" s="104"/>
+      <c r="C107" s="104"/>
+      <c r="D107" s="104"/>
+      <c r="E107" s="104"/>
+      <c r="F107" s="104"/>
+      <c r="G107" s="104"/>
+      <c r="H107" s="104"/>
+      <c r="I107" s="105"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A108" s="102" t="s">
+      <c r="A108" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="B108" s="70"/>
-      <c r="C108" s="70"/>
-      <c r="D108" s="70"/>
-      <c r="E108" s="70"/>
-      <c r="F108" s="70"/>
-      <c r="G108" s="70"/>
-      <c r="H108" s="70"/>
-      <c r="I108" s="103"/>
+      <c r="B108" s="104"/>
+      <c r="C108" s="104"/>
+      <c r="D108" s="104"/>
+      <c r="E108" s="104"/>
+      <c r="F108" s="104"/>
+      <c r="G108" s="104"/>
+      <c r="H108" s="104"/>
+      <c r="I108" s="105"/>
     </row>
     <row r="109" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="86"/>
-      <c r="B109" s="87"/>
-      <c r="C109" s="87"/>
-      <c r="D109" s="87"/>
-      <c r="E109" s="87"/>
-      <c r="F109" s="88"/>
-      <c r="G109" s="104" t="s">
+      <c r="A109" s="87"/>
+      <c r="B109" s="88"/>
+      <c r="C109" s="88"/>
+      <c r="D109" s="88"/>
+      <c r="E109" s="88"/>
+      <c r="F109" s="89"/>
+      <c r="G109" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="H109" s="105"/>
+      <c r="H109" s="76"/>
       <c r="I109" s="20">
         <f>SUM(J92:J97)</f>
         <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="86"/>
-      <c r="B110" s="87"/>
-      <c r="C110" s="87"/>
-      <c r="D110" s="87"/>
-      <c r="E110" s="87"/>
-      <c r="F110" s="88"/>
-      <c r="G110" s="104" t="s">
+      <c r="A110" s="87"/>
+      <c r="B110" s="88"/>
+      <c r="C110" s="88"/>
+      <c r="D110" s="88"/>
+      <c r="E110" s="88"/>
+      <c r="F110" s="89"/>
+      <c r="G110" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="H110" s="105"/>
+      <c r="H110" s="76"/>
       <c r="I110" s="20">
         <f>SUM(J98:J99)</f>
         <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="86"/>
-      <c r="B111" s="87"/>
-      <c r="C111" s="87"/>
-      <c r="D111" s="87"/>
-      <c r="E111" s="87"/>
-      <c r="F111" s="88"/>
-      <c r="G111" s="104" t="s">
+      <c r="A111" s="87"/>
+      <c r="B111" s="88"/>
+      <c r="C111" s="88"/>
+      <c r="D111" s="88"/>
+      <c r="E111" s="88"/>
+      <c r="F111" s="89"/>
+      <c r="G111" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="H111" s="105"/>
+      <c r="H111" s="76"/>
       <c r="I111" s="20">
         <f>I109+I110</f>
         <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="111" t="s">
+      <c r="A112" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="B112" s="112"/>
-      <c r="C112" s="112"/>
-      <c r="D112" s="112"/>
-      <c r="E112" s="112"/>
-      <c r="F112" s="112"/>
-      <c r="G112" s="112"/>
-      <c r="H112" s="112"/>
+      <c r="B112" s="81"/>
+      <c r="C112" s="81"/>
+      <c r="D112" s="81"/>
+      <c r="E112" s="81"/>
+      <c r="F112" s="81"/>
+      <c r="G112" s="81"/>
+      <c r="H112" s="81"/>
       <c r="I112" s="21" t="str">
         <f>C123</f>
         <v>Reduzir a complexidade</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="109" t="s">
+      <c r="A113" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="B113" s="83"/>
-      <c r="C113" s="83"/>
-      <c r="D113" s="83"/>
-      <c r="E113" s="83"/>
-      <c r="F113" s="83"/>
-      <c r="G113" s="83"/>
-      <c r="H113" s="83"/>
-      <c r="I113" s="110"/>
+      <c r="B113" s="78"/>
+      <c r="C113" s="78"/>
+      <c r="D113" s="78"/>
+      <c r="E113" s="78"/>
+      <c r="F113" s="78"/>
+      <c r="G113" s="78"/>
+      <c r="H113" s="78"/>
+      <c r="I113" s="79"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="100" t="s">
+      <c r="A114" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B114" s="84"/>
-      <c r="C114" s="84"/>
-      <c r="D114" s="84"/>
-      <c r="E114" s="84"/>
-      <c r="F114" s="84"/>
-      <c r="G114" s="84"/>
-      <c r="H114" s="84"/>
-      <c r="I114" s="101"/>
+      <c r="B114" s="99"/>
+      <c r="C114" s="99"/>
+      <c r="D114" s="99"/>
+      <c r="E114" s="99"/>
+      <c r="F114" s="99"/>
+      <c r="G114" s="99"/>
+      <c r="H114" s="99"/>
+      <c r="I114" s="100"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" s="100" t="s">
+      <c r="A115" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="B115" s="84"/>
-      <c r="C115" s="84"/>
-      <c r="D115" s="84"/>
-      <c r="E115" s="84"/>
-      <c r="F115" s="84"/>
-      <c r="G115" s="84"/>
-      <c r="H115" s="84"/>
-      <c r="I115" s="101"/>
+      <c r="B115" s="99"/>
+      <c r="C115" s="99"/>
+      <c r="D115" s="99"/>
+      <c r="E115" s="99"/>
+      <c r="F115" s="99"/>
+      <c r="G115" s="99"/>
+      <c r="H115" s="99"/>
+      <c r="I115" s="100"/>
     </row>
     <row r="116" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="106" t="s">
@@ -3788,16 +3803,16 @@
       <c r="I116" s="108"/>
     </row>
     <row r="121" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A121" s="73" t="s">
+      <c r="A121" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="B121" s="83"/>
-      <c r="C121" s="83"/>
-      <c r="D121" s="83"/>
-      <c r="E121" s="83"/>
-      <c r="F121" s="83"/>
-      <c r="G121" s="83"/>
-      <c r="H121" s="83"/>
+      <c r="B121" s="78"/>
+      <c r="C121" s="78"/>
+      <c r="D121" s="78"/>
+      <c r="E121" s="78"/>
+      <c r="F121" s="78"/>
+      <c r="G121" s="78"/>
+      <c r="H121" s="78"/>
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="46" t="s">
@@ -3887,16 +3902,16 @@
       <c r="H125" s="3"/>
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="83" t="s">
+      <c r="A126" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="B126" s="83"/>
-      <c r="C126" s="83"/>
-      <c r="D126" s="83"/>
-      <c r="E126" s="83"/>
-      <c r="F126" s="83"/>
-      <c r="G126" s="83"/>
-      <c r="H126" s="83"/>
+      <c r="B126" s="78"/>
+      <c r="C126" s="78"/>
+      <c r="D126" s="78"/>
+      <c r="E126" s="78"/>
+      <c r="F126" s="78"/>
+      <c r="G126" s="78"/>
+      <c r="H126" s="78"/>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="46" t="s">
@@ -3987,16 +4002,16 @@
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A131" s="83" t="s">
+      <c r="A131" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="B131" s="83"/>
-      <c r="C131" s="83"/>
-      <c r="D131" s="83"/>
-      <c r="E131" s="83"/>
-      <c r="F131" s="83"/>
-      <c r="G131" s="83"/>
-      <c r="H131" s="83"/>
+      <c r="B131" s="78"/>
+      <c r="C131" s="78"/>
+      <c r="D131" s="78"/>
+      <c r="E131" s="78"/>
+      <c r="F131" s="78"/>
+      <c r="G131" s="78"/>
+      <c r="H131" s="78"/>
     </row>
     <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="46" t="s">
@@ -4101,19 +4116,59 @@
     </row>
   </sheetData>
   <mergeCells count="101">
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="A113:I113"/>
-    <mergeCell ref="A112:H112"/>
-    <mergeCell ref="A104:I104"/>
-    <mergeCell ref="A105:I105"/>
-    <mergeCell ref="A106:I106"/>
-    <mergeCell ref="A109:F109"/>
-    <mergeCell ref="A110:F110"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="A68:I68"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="A64:I64"/>
+    <mergeCell ref="A65:I65"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="A100:H100"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="A85:I85"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="A87:I87"/>
+    <mergeCell ref="A88:I88"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="A89:I89"/>
+    <mergeCell ref="A90:I90"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="B79:E79"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A121:H121"/>
@@ -4138,31 +4193,20 @@
     <mergeCell ref="H82:I82"/>
     <mergeCell ref="A83:G83"/>
     <mergeCell ref="H83:I83"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A113:I113"/>
+    <mergeCell ref="A112:H112"/>
+    <mergeCell ref="A104:I104"/>
+    <mergeCell ref="A105:I105"/>
+    <mergeCell ref="A106:I106"/>
+    <mergeCell ref="A109:F109"/>
+    <mergeCell ref="A110:F110"/>
     <mergeCell ref="A111:F111"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="A100:H100"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="A85:I85"/>
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="A87:I87"/>
-    <mergeCell ref="A88:I88"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="A89:I89"/>
-    <mergeCell ref="A90:I90"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="B79:E79"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="B80:E80"/>
     <mergeCell ref="H80:I80"/>
@@ -4173,35 +4217,6 @@
     <mergeCell ref="B70:E70"/>
     <mergeCell ref="H70:I70"/>
     <mergeCell ref="A67:I67"/>
-    <mergeCell ref="A68:I68"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="A65:I65"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B33:H33"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="4">

</xml_diff>